<commit_message>
full stack with JSON database
</commit_message>
<xml_diff>
--- a/server/Context.xlsx
+++ b/server/Context.xlsx
@@ -397,13 +397,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>www.google.com</v>
+      </c>
+      <c r="B1" t="str">
+        <v>a</v>
+      </c>
+      <c r="C1" t="str">
+        <v>b</v>
+      </c>
+      <c r="D1" t="str">
+        <v>c</v>
+      </c>
+      <c r="E1" t="str">
+        <v>d</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>www.google.com</v>
+      </c>
+      <c r="B2" t="str">
+        <v>5</v>
+      </c>
+      <c r="C2" t="str">
+        <v>6</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>